<commit_message>
Use new (synthetic) OECM Oil and Gas sectors
Instead of synthesizing Oil and Gas ourselves for ITR_UI.py, use the newly synthesized sector coming from itr-data-pipeline.

Also, resync ITR_DV.py with ITR_UI.py (until we re-unify the two) and note that with the new Oil & Gas sector we now have 69 tests in test_base_providers.py, not 66.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20230524 ITR V2 SBTi.xlsx
+++ b/examples/data/20230524 ITR V2 SBTi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92DFEB-9ABA-6D41-B54E-5B13E77042CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7137EF1C-0AC3-6142-BFD9-AAC461B42DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40620" windowHeight="22280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -21,7 +21,20 @@
     <sheet name="Portfolio" sheetId="5" r:id="rId6"/>
     <sheet name="User Notes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1965,7 +1978,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2126,6 +2139,7 @@
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2150,12 +2164,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3375,9 +3383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -4304,10 +4310,10 @@
   <dimension ref="A1:Q278"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C242" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomRight" activeCell="H95" sqref="H95:H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4380,13 +4386,13 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="81" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="49" t="s">
@@ -4404,9 +4410,9 @@
       <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="76"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="80"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="49" t="s">
         <v>196</v>
       </c>
@@ -4417,7 +4423,7 @@
         <v>207</v>
       </c>
       <c r="H3" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I3" s="40">
         <v>1806880.79033897</v>
@@ -4434,9 +4440,9 @@
       <c r="P3" s="40"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="76"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="80"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="81"/>
       <c r="D4" s="49" t="s">
         <v>257</v>
       </c>
@@ -4450,7 +4456,7 @@
         <v>209</v>
       </c>
       <c r="H4" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I4" s="66">
         <v>0.292034636322417</v>
@@ -4467,9 +4473,9 @@
       <c r="P4" s="66"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="76"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="80"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="49" t="s">
         <v>196</v>
       </c>
@@ -4480,7 +4486,7 @@
         <v>207</v>
       </c>
       <c r="H5" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I5" s="40">
         <v>9913677.1400000006</v>
@@ -4497,9 +4503,9 @@
       <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="76"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="80"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="49" t="s">
         <v>257</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>209</v>
       </c>
       <c r="H6" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I6" s="66">
         <v>0.369901153033176</v>
@@ -4530,9 +4536,9 @@
       <c r="P6" s="66"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="76"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="80"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="49" t="s">
         <v>199</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>208</v>
       </c>
       <c r="H7" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="K7" s="54"/>
       <c r="L7" s="55"/>
@@ -4553,9 +4559,9 @@
       <c r="P7" s="55"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="76"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="80"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="49" t="s">
         <v>200</v>
       </c>
@@ -4566,7 +4572,7 @@
         <v>207</v>
       </c>
       <c r="H8" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="K8" s="54"/>
       <c r="L8" s="55"/>
@@ -4580,9 +4586,9 @@
       <c r="P8" s="40"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="49" t="s">
         <v>202</v>
       </c>
@@ -4593,7 +4599,7 @@
         <v>271</v>
       </c>
       <c r="H9" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I9" s="61">
         <v>222922</v>
@@ -4610,9 +4616,9 @@
       <c r="P9" s="55"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="80"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="81"/>
       <c r="D10" s="49" t="s">
         <v>202</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>57</v>
       </c>
       <c r="H10" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I10" s="61">
         <f>SUM(I11:I21)</f>
@@ -4646,9 +4652,9 @@
       <c r="P10" s="55"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="76"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="80"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="49" t="s">
         <v>215</v>
       </c>
@@ -4662,7 +4668,7 @@
         <v>57</v>
       </c>
       <c r="H11" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I11" s="55"/>
       <c r="J11" s="55"/>
@@ -4674,9 +4680,9 @@
       <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="76"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="80"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="49" t="s">
         <v>215</v>
       </c>
@@ -4690,7 +4696,7 @@
         <v>57</v>
       </c>
       <c r="H12" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I12" s="55">
         <v>2181551</v>
@@ -4708,9 +4714,9 @@
       <c r="P12" s="55"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="76"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="80"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="81"/>
       <c r="D13" s="49" t="s">
         <v>215</v>
       </c>
@@ -4724,7 +4730,7 @@
         <v>57</v>
       </c>
       <c r="H13" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I13" s="55"/>
       <c r="J13" s="55"/>
@@ -4736,9 +4742,9 @@
       <c r="P13" s="55"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="76"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="80"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="49" t="s">
         <v>215</v>
       </c>
@@ -4752,7 +4758,7 @@
         <v>57</v>
       </c>
       <c r="H14" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I14" s="55">
         <v>80129</v>
@@ -4770,9 +4776,9 @@
       <c r="P14" s="55"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="76"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="80"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="49" t="s">
         <v>215</v>
       </c>
@@ -4786,7 +4792,7 @@
         <v>57</v>
       </c>
       <c r="H15" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I15" s="55"/>
       <c r="J15" s="55"/>
@@ -4798,9 +4804,9 @@
       <c r="P15" s="55"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="76"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="80"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="49" t="s">
         <v>215</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>57</v>
       </c>
       <c r="H16" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I16" s="55"/>
       <c r="J16" s="55"/>
@@ -4826,9 +4832,9 @@
       <c r="P16" s="55"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="76"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="80"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="49" t="s">
         <v>215</v>
       </c>
@@ -4842,7 +4848,7 @@
         <v>57</v>
       </c>
       <c r="H17" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="55"/>
@@ -4854,9 +4860,9 @@
       <c r="P17" s="55"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="76"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="80"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="49" t="s">
         <v>215</v>
       </c>
@@ -4870,7 +4876,7 @@
         <v>57</v>
       </c>
       <c r="H18" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I18" s="55"/>
       <c r="J18" s="55"/>
@@ -4882,9 +4888,9 @@
       <c r="P18" s="55"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="76"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="80"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="49" t="s">
         <v>215</v>
       </c>
@@ -4898,7 +4904,7 @@
         <v>57</v>
       </c>
       <c r="H19" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I19" s="55"/>
       <c r="J19" s="55"/>
@@ -4914,9 +4920,9 @@
       <c r="P19" s="55"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="76"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="80"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="49" t="s">
         <v>215</v>
       </c>
@@ -4930,7 +4936,7 @@
         <v>57</v>
       </c>
       <c r="H20" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
@@ -4946,9 +4952,9 @@
       <c r="P20" s="55"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="76"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="80"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="49" t="s">
         <v>215</v>
       </c>
@@ -4962,7 +4968,7 @@
         <v>57</v>
       </c>
       <c r="H21" s="48">
-        <v>44756</v>
+        <v>43967</v>
       </c>
       <c r="I21" s="55">
         <v>3925534</v>
@@ -4980,9 +4986,9 @@
       <c r="P21" s="55"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="76"/>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="81"/>
       <c r="D22" s="49" t="s">
         <v>227</v>
       </c>
@@ -4997,13 +5003,13 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="81" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="49" t="s">
@@ -5021,9 +5027,9 @@
       <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="76"/>
-      <c r="B24" s="78"/>
-      <c r="C24" s="80"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="81"/>
       <c r="D24" s="49" t="s">
         <v>196</v>
       </c>
@@ -5051,9 +5057,9 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="76"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="80"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="49" t="s">
         <v>257</v>
       </c>
@@ -5084,9 +5090,9 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="76"/>
-      <c r="B26" s="78"/>
-      <c r="C26" s="80"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="49" t="s">
         <v>196</v>
       </c>
@@ -5114,9 +5120,9 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="76"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="80"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="49" t="s">
         <v>257</v>
       </c>
@@ -5147,9 +5153,9 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="76"/>
-      <c r="B28" s="78"/>
-      <c r="C28" s="80"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="81"/>
       <c r="D28" s="49" t="s">
         <v>199</v>
       </c>
@@ -5170,9 +5176,9 @@
       <c r="P28" s="55"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="76"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="80"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="81"/>
       <c r="D29" s="49" t="s">
         <v>200</v>
       </c>
@@ -5197,9 +5203,9 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="76"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="80"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="81"/>
       <c r="D30" s="49" t="s">
         <v>261</v>
       </c>
@@ -5227,9 +5233,9 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="76"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="80"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="81"/>
       <c r="D31" s="49" t="s">
         <v>261</v>
       </c>
@@ -5254,9 +5260,9 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="76"/>
-      <c r="B32" s="78"/>
-      <c r="C32" s="80"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="81"/>
       <c r="D32" s="49" t="s">
         <v>202</v>
       </c>
@@ -5287,9 +5293,9 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="76"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="80"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="81"/>
       <c r="D33" s="49" t="s">
         <v>202</v>
       </c>
@@ -5323,9 +5329,9 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="76"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="80"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="81"/>
       <c r="D34" s="49" t="s">
         <v>215</v>
       </c>
@@ -5355,9 +5361,9 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="76"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="80"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="81"/>
       <c r="D35" s="49" t="s">
         <v>215</v>
       </c>
@@ -5389,9 +5395,9 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="76"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="80"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="81"/>
       <c r="D36" s="49" t="s">
         <v>215</v>
       </c>
@@ -5421,9 +5427,9 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="76"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="80"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="81"/>
       <c r="D37" s="49" t="s">
         <v>215</v>
       </c>
@@ -5455,9 +5461,9 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="76"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="80"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="49" t="s">
         <v>215</v>
       </c>
@@ -5483,9 +5489,9 @@
       <c r="P38" s="55"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="76"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="80"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="79"/>
+      <c r="C39" s="81"/>
       <c r="D39" s="49" t="s">
         <v>215</v>
       </c>
@@ -5515,9 +5521,9 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="76"/>
-      <c r="B40" s="78"/>
-      <c r="C40" s="80"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="79"/>
+      <c r="C40" s="81"/>
       <c r="D40" s="49" t="s">
         <v>215</v>
       </c>
@@ -5547,9 +5553,9 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="76"/>
-      <c r="B41" s="78"/>
-      <c r="C41" s="80"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="79"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="49" t="s">
         <v>215</v>
       </c>
@@ -5579,9 +5585,9 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="76"/>
-      <c r="B42" s="78"/>
-      <c r="C42" s="80"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="79"/>
+      <c r="C42" s="81"/>
       <c r="D42" s="49" t="s">
         <v>215</v>
       </c>
@@ -5611,9 +5617,9 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="76"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="80"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="81"/>
       <c r="D43" s="49" t="s">
         <v>215</v>
       </c>
@@ -5643,9 +5649,9 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="76"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="80"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="81"/>
       <c r="D44" s="49" t="s">
         <v>215</v>
       </c>
@@ -5677,9 +5683,9 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="76"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="80"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="81"/>
       <c r="D45" s="49" t="s">
         <v>227</v>
       </c>
@@ -5694,9 +5700,9 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="76"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="80"/>
+      <c r="A46" s="77"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="81"/>
       <c r="D46" s="49" t="s">
         <v>203</v>
       </c>
@@ -5713,13 +5719,13 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" s="76" t="s">
+      <c r="A47" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="77" t="s">
+      <c r="B47" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="80" t="s">
+      <c r="C47" s="81" t="s">
         <v>67</v>
       </c>
       <c r="D47" s="49" t="s">
@@ -5747,9 +5753,9 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="76"/>
-      <c r="B48" s="78"/>
-      <c r="C48" s="80"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="79"/>
+      <c r="C48" s="81"/>
       <c r="D48" s="49" t="s">
         <v>197</v>
       </c>
@@ -5778,9 +5784,9 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="76"/>
-      <c r="B49" s="78"/>
-      <c r="C49" s="80"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="79"/>
+      <c r="C49" s="81"/>
       <c r="D49" s="49" t="s">
         <v>199</v>
       </c>
@@ -5809,9 +5815,9 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="76"/>
-      <c r="B50" s="78"/>
-      <c r="C50" s="80"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="81"/>
       <c r="D50" s="49" t="s">
         <v>200</v>
       </c>
@@ -5840,9 +5846,9 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="76"/>
-      <c r="B51" s="78"/>
-      <c r="C51" s="80"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="81"/>
       <c r="D51" s="49" t="s">
         <v>202</v>
       </c>
@@ -5868,9 +5874,9 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="76"/>
-      <c r="B52" s="79"/>
-      <c r="C52" s="80"/>
+      <c r="A52" s="77"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="81"/>
       <c r="D52" s="49" t="s">
         <v>203</v>
       </c>
@@ -5891,13 +5897,13 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="76" t="s">
+      <c r="A53" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="80" t="s">
+      <c r="C53" s="81" t="s">
         <v>71</v>
       </c>
       <c r="D53" s="49" t="s">
@@ -5923,9 +5929,9 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="76"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="80"/>
+      <c r="A54" s="77"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="81"/>
       <c r="D54" s="49" t="s">
         <v>257</v>
       </c>
@@ -5949,9 +5955,9 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="76"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="80"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="81"/>
       <c r="D55" s="49" t="s">
         <v>197</v>
       </c>
@@ -5978,9 +5984,9 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="76"/>
-      <c r="B56" s="78"/>
-      <c r="C56" s="80"/>
+      <c r="A56" s="77"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="81"/>
       <c r="D56" s="49" t="s">
         <v>197</v>
       </c>
@@ -6007,9 +6013,9 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="76"/>
-      <c r="B57" s="78"/>
-      <c r="C57" s="80"/>
+      <c r="A57" s="77"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="81"/>
       <c r="D57" s="49" t="s">
         <v>200</v>
       </c>
@@ -6039,9 +6045,9 @@
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="76"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="80"/>
+      <c r="A58" s="77"/>
+      <c r="B58" s="79"/>
+      <c r="C58" s="81"/>
       <c r="D58" s="49" t="s">
         <v>200</v>
       </c>
@@ -6071,9 +6077,9 @@
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="76"/>
-      <c r="B59" s="78"/>
-      <c r="C59" s="80"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="81"/>
       <c r="D59" s="49" t="s">
         <v>200</v>
       </c>
@@ -6100,9 +6106,9 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="76"/>
-      <c r="B60" s="78"/>
-      <c r="C60" s="80"/>
+      <c r="A60" s="77"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="81"/>
       <c r="D60" s="49" t="s">
         <v>200</v>
       </c>
@@ -6132,9 +6138,9 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="76"/>
-      <c r="B61" s="78"/>
-      <c r="C61" s="80"/>
+      <c r="A61" s="77"/>
+      <c r="B61" s="79"/>
+      <c r="C61" s="81"/>
       <c r="D61" s="49" t="s">
         <v>200</v>
       </c>
@@ -6164,9 +6170,9 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" s="76"/>
-      <c r="B62" s="78"/>
-      <c r="C62" s="80"/>
+      <c r="A62" s="77"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="81"/>
       <c r="D62" s="49" t="s">
         <v>200</v>
       </c>
@@ -6196,9 +6202,9 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="76"/>
-      <c r="B63" s="78"/>
-      <c r="C63" s="80"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="79"/>
+      <c r="C63" s="81"/>
       <c r="D63" s="49" t="s">
         <v>202</v>
       </c>
@@ -6228,9 +6234,9 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A64" s="76"/>
-      <c r="B64" s="78"/>
-      <c r="C64" s="80"/>
+      <c r="A64" s="77"/>
+      <c r="B64" s="79"/>
+      <c r="C64" s="81"/>
       <c r="D64" s="49" t="s">
         <v>202</v>
       </c>
@@ -6257,9 +6263,9 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65" s="76"/>
-      <c r="B65" s="79"/>
-      <c r="C65" s="80"/>
+      <c r="A65" s="77"/>
+      <c r="B65" s="80"/>
+      <c r="C65" s="81"/>
       <c r="D65" s="49" t="s">
         <v>203</v>
       </c>
@@ -6276,13 +6282,13 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66" s="76" t="s">
+      <c r="A66" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="77" t="s">
+      <c r="B66" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="80" t="s">
+      <c r="C66" s="81" t="s">
         <v>71</v>
       </c>
       <c r="D66" s="49" t="s">
@@ -6308,9 +6314,9 @@
       <c r="P66" s="55"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67" s="76"/>
-      <c r="B67" s="78"/>
-      <c r="C67" s="80"/>
+      <c r="A67" s="77"/>
+      <c r="B67" s="79"/>
+      <c r="C67" s="81"/>
       <c r="D67" s="49" t="s">
         <v>257</v>
       </c>
@@ -6334,9 +6340,9 @@
       <c r="P67" s="55"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68" s="76"/>
-      <c r="B68" s="78"/>
-      <c r="C68" s="80"/>
+      <c r="A68" s="77"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="81"/>
       <c r="D68" s="49" t="s">
         <v>197</v>
       </c>
@@ -6366,9 +6372,9 @@
       <c r="P68" s="55"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A69" s="76"/>
-      <c r="B69" s="78"/>
-      <c r="C69" s="80"/>
+      <c r="A69" s="77"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="81"/>
       <c r="D69" s="49" t="s">
         <v>197</v>
       </c>
@@ -6395,9 +6401,9 @@
       <c r="P69" s="55"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A70" s="76"/>
-      <c r="B70" s="78"/>
-      <c r="C70" s="80"/>
+      <c r="A70" s="77"/>
+      <c r="B70" s="79"/>
+      <c r="C70" s="81"/>
       <c r="D70" s="49" t="s">
         <v>200</v>
       </c>
@@ -6430,9 +6436,9 @@
       <c r="P70" s="55"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A71" s="76"/>
-      <c r="B71" s="78"/>
-      <c r="C71" s="80"/>
+      <c r="A71" s="77"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="81"/>
       <c r="D71" s="49" t="s">
         <v>200</v>
       </c>
@@ -6459,9 +6465,9 @@
       <c r="P71" s="55"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72" s="76"/>
-      <c r="B72" s="78"/>
-      <c r="C72" s="80"/>
+      <c r="A72" s="77"/>
+      <c r="B72" s="79"/>
+      <c r="C72" s="81"/>
       <c r="D72" s="49" t="s">
         <v>200</v>
       </c>
@@ -6482,9 +6488,9 @@
       <c r="P72" s="55"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73" s="76"/>
-      <c r="B73" s="78"/>
-      <c r="C73" s="80"/>
+      <c r="A73" s="77"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="81"/>
       <c r="D73" s="49" t="s">
         <v>200</v>
       </c>
@@ -6514,9 +6520,9 @@
       <c r="P73" s="55"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A74" s="76"/>
-      <c r="B74" s="78"/>
-      <c r="C74" s="80"/>
+      <c r="A74" s="77"/>
+      <c r="B74" s="79"/>
+      <c r="C74" s="81"/>
       <c r="D74" s="49" t="s">
         <v>200</v>
       </c>
@@ -6546,9 +6552,9 @@
       <c r="P74" s="55"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A75" s="76"/>
-      <c r="B75" s="78"/>
-      <c r="C75" s="80"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="79"/>
+      <c r="C75" s="81"/>
       <c r="D75" s="49" t="s">
         <v>200</v>
       </c>
@@ -6578,9 +6584,9 @@
       <c r="P75" s="55"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A76" s="76"/>
-      <c r="B76" s="78"/>
-      <c r="C76" s="80"/>
+      <c r="A76" s="77"/>
+      <c r="B76" s="79"/>
+      <c r="C76" s="81"/>
       <c r="D76" s="49" t="s">
         <v>202</v>
       </c>
@@ -6610,9 +6616,9 @@
       <c r="P76" s="55"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77" s="76"/>
-      <c r="B77" s="78"/>
-      <c r="C77" s="80"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="79"/>
+      <c r="C77" s="81"/>
       <c r="D77" s="49" t="s">
         <v>202</v>
       </c>
@@ -6639,9 +6645,9 @@
       <c r="P77" s="55"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="76"/>
-      <c r="B78" s="79"/>
-      <c r="C78" s="80"/>
+      <c r="A78" s="77"/>
+      <c r="B78" s="80"/>
+      <c r="C78" s="81"/>
       <c r="D78" s="49" t="s">
         <v>203</v>
       </c>
@@ -6658,13 +6664,13 @@
       <c r="P78" s="57"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79" s="81" t="s">
+      <c r="A79" s="82" t="s">
         <v>311</v>
       </c>
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="C79" s="77" t="s">
+      <c r="C79" s="78" t="s">
         <v>313</v>
       </c>
       <c r="D79" s="49" t="s">
@@ -6694,9 +6700,9 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80" s="82"/>
-      <c r="B80" s="78"/>
-      <c r="C80" s="78"/>
+      <c r="A80" s="83"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="79"/>
       <c r="D80" s="49" t="s">
         <v>197</v>
       </c>
@@ -6724,9 +6730,9 @@
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81" s="82"/>
-      <c r="B81" s="78"/>
-      <c r="C81" s="78"/>
+      <c r="A81" s="83"/>
+      <c r="B81" s="79"/>
+      <c r="C81" s="79"/>
       <c r="D81" s="58" t="s">
         <v>200</v>
       </c>
@@ -6755,9 +6761,9 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82" s="82"/>
-      <c r="B82" s="78"/>
-      <c r="C82" s="78"/>
+      <c r="A82" s="83"/>
+      <c r="B82" s="79"/>
+      <c r="C82" s="79"/>
       <c r="D82" s="49" t="s">
         <v>200</v>
       </c>
@@ -6785,9 +6791,9 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="82"/>
-      <c r="B83" s="78"/>
-      <c r="C83" s="78"/>
+      <c r="A83" s="83"/>
+      <c r="B83" s="79"/>
+      <c r="C83" s="79"/>
       <c r="D83" s="49" t="s">
         <v>200</v>
       </c>
@@ -6815,9 +6821,9 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" s="82"/>
-      <c r="B84" s="78"/>
-      <c r="C84" s="78"/>
+      <c r="A84" s="83"/>
+      <c r="B84" s="79"/>
+      <c r="C84" s="79"/>
       <c r="D84" s="49" t="s">
         <v>202</v>
       </c>
@@ -6845,9 +6851,9 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="82"/>
-      <c r="B85" s="78"/>
-      <c r="C85" s="78"/>
+      <c r="A85" s="83"/>
+      <c r="B85" s="79"/>
+      <c r="C85" s="79"/>
       <c r="D85" s="49" t="s">
         <v>202</v>
       </c>
@@ -6875,9 +6881,9 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" s="83"/>
-      <c r="B86" s="79"/>
-      <c r="C86" s="79"/>
+      <c r="A86" s="84"/>
+      <c r="B86" s="80"/>
+      <c r="C86" s="80"/>
       <c r="D86" s="49" t="s">
         <v>203</v>
       </c>
@@ -6895,13 +6901,13 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87" s="81" t="s">
+      <c r="A87" s="82" t="s">
         <v>311</v>
       </c>
-      <c r="B87" s="77" t="s">
+      <c r="B87" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="C87" s="77" t="s">
+      <c r="C87" s="78" t="s">
         <v>313</v>
       </c>
       <c r="D87" s="49" t="s">
@@ -6914,7 +6920,7 @@
         <v>208</v>
       </c>
       <c r="H87" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K87" s="54"/>
       <c r="L87" s="55"/>
@@ -6930,9 +6936,9 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A88" s="82"/>
-      <c r="B88" s="78"/>
-      <c r="C88" s="78"/>
+      <c r="A88" s="83"/>
+      <c r="B88" s="79"/>
+      <c r="C88" s="79"/>
       <c r="D88" s="49" t="s">
         <v>197</v>
       </c>
@@ -6943,7 +6949,7 @@
         <v>208</v>
       </c>
       <c r="H88" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K88" s="54"/>
       <c r="L88" s="55"/>
@@ -6959,9 +6965,9 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89" s="82"/>
-      <c r="B89" s="78"/>
-      <c r="C89" s="78"/>
+      <c r="A89" s="83"/>
+      <c r="B89" s="79"/>
+      <c r="C89" s="79"/>
       <c r="D89" s="58" t="s">
         <v>200</v>
       </c>
@@ -6970,7 +6976,7 @@
         <v>208</v>
       </c>
       <c r="H89" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="I89" s="61" t="s">
         <v>286</v>
@@ -6989,9 +6995,9 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90" s="82"/>
-      <c r="B90" s="78"/>
-      <c r="C90" s="78"/>
+      <c r="A90" s="83"/>
+      <c r="B90" s="79"/>
+      <c r="C90" s="79"/>
       <c r="D90" s="49" t="s">
         <v>200</v>
       </c>
@@ -7002,7 +7008,7 @@
         <v>208</v>
       </c>
       <c r="H90" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K90" s="54"/>
       <c r="L90" s="55"/>
@@ -7018,9 +7024,9 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91" s="82"/>
-      <c r="B91" s="78"/>
-      <c r="C91" s="78"/>
+      <c r="A91" s="83"/>
+      <c r="B91" s="79"/>
+      <c r="C91" s="79"/>
       <c r="D91" s="49" t="s">
         <v>200</v>
       </c>
@@ -7031,7 +7037,7 @@
         <v>208</v>
       </c>
       <c r="H91" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K91" s="54"/>
       <c r="L91" s="55"/>
@@ -7047,9 +7053,9 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92" s="82"/>
-      <c r="B92" s="78"/>
-      <c r="C92" s="78"/>
+      <c r="A92" s="83"/>
+      <c r="B92" s="79"/>
+      <c r="C92" s="79"/>
       <c r="D92" s="49" t="s">
         <v>202</v>
       </c>
@@ -7060,7 +7066,7 @@
         <v>55</v>
       </c>
       <c r="H92" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K92" s="54"/>
       <c r="L92" s="55"/>
@@ -7076,9 +7082,9 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93" s="82"/>
-      <c r="B93" s="78"/>
-      <c r="C93" s="78"/>
+      <c r="A93" s="83"/>
+      <c r="B93" s="79"/>
+      <c r="C93" s="79"/>
       <c r="D93" s="49" t="s">
         <v>202</v>
       </c>
@@ -7089,7 +7095,7 @@
         <v>55</v>
       </c>
       <c r="H93" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K93" s="54"/>
       <c r="L93" s="55"/>
@@ -7105,14 +7111,14 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94" s="83"/>
-      <c r="B94" s="79"/>
-      <c r="C94" s="79"/>
+      <c r="A94" s="84"/>
+      <c r="B94" s="80"/>
+      <c r="C94" s="80"/>
       <c r="D94" s="49" t="s">
         <v>203</v>
       </c>
       <c r="H94" s="48">
-        <v>44958</v>
+        <v>44617</v>
       </c>
       <c r="K94" s="54"/>
       <c r="L94" s="55"/>
@@ -7124,13 +7130,13 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A95" s="81" t="s">
+      <c r="A95" s="82" t="s">
         <v>311</v>
       </c>
-      <c r="B95" s="77" t="s">
+      <c r="B95" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="C95" s="77" t="s">
+      <c r="C95" s="78" t="s">
         <v>313</v>
       </c>
       <c r="D95" s="49" t="s">
@@ -7143,7 +7149,7 @@
         <v>208</v>
       </c>
       <c r="H95" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K95" s="54"/>
       <c r="L95" s="55"/>
@@ -7159,9 +7165,9 @@
       <c r="P95" s="55"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96" s="82"/>
-      <c r="B96" s="78"/>
-      <c r="C96" s="78"/>
+      <c r="A96" s="83"/>
+      <c r="B96" s="79"/>
+      <c r="C96" s="79"/>
       <c r="D96" s="49" t="s">
         <v>197</v>
       </c>
@@ -7172,7 +7178,7 @@
         <v>208</v>
       </c>
       <c r="H96" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K96" s="54"/>
       <c r="L96" s="55"/>
@@ -7188,9 +7194,9 @@
       <c r="P96" s="55"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="82"/>
-      <c r="B97" s="78"/>
-      <c r="C97" s="78"/>
+      <c r="A97" s="83"/>
+      <c r="B97" s="79"/>
+      <c r="C97" s="79"/>
       <c r="D97" s="58" t="s">
         <v>200</v>
       </c>
@@ -7199,7 +7205,7 @@
         <v>208</v>
       </c>
       <c r="H97" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="I97" s="61" t="s">
         <v>286</v>
@@ -7218,9 +7224,9 @@
       <c r="P97" s="55"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A98" s="82"/>
-      <c r="B98" s="78"/>
-      <c r="C98" s="78"/>
+      <c r="A98" s="83"/>
+      <c r="B98" s="79"/>
+      <c r="C98" s="79"/>
       <c r="D98" s="49" t="s">
         <v>200</v>
       </c>
@@ -7231,7 +7237,7 @@
         <v>208</v>
       </c>
       <c r="H98" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K98" s="54"/>
       <c r="L98" s="55"/>
@@ -7247,9 +7253,9 @@
       <c r="P98" s="55"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="82"/>
-      <c r="B99" s="78"/>
-      <c r="C99" s="78"/>
+      <c r="A99" s="83"/>
+      <c r="B99" s="79"/>
+      <c r="C99" s="79"/>
       <c r="D99" s="49" t="s">
         <v>200</v>
       </c>
@@ -7260,7 +7266,7 @@
         <v>208</v>
       </c>
       <c r="H99" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K99" s="54"/>
       <c r="L99" s="55"/>
@@ -7276,9 +7282,9 @@
       <c r="P99" s="55"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A100" s="82"/>
-      <c r="B100" s="78"/>
-      <c r="C100" s="78"/>
+      <c r="A100" s="83"/>
+      <c r="B100" s="79"/>
+      <c r="C100" s="79"/>
       <c r="D100" s="49" t="s">
         <v>202</v>
       </c>
@@ -7289,7 +7295,7 @@
         <v>55</v>
       </c>
       <c r="H100" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K100" s="54"/>
       <c r="L100" s="55"/>
@@ -7305,9 +7311,9 @@
       <c r="P100" s="55"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A101" s="82"/>
-      <c r="B101" s="78"/>
-      <c r="C101" s="78"/>
+      <c r="A101" s="83"/>
+      <c r="B101" s="79"/>
+      <c r="C101" s="79"/>
       <c r="D101" s="49" t="s">
         <v>202</v>
       </c>
@@ -7318,7 +7324,7 @@
         <v>55</v>
       </c>
       <c r="H101" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K101" s="54"/>
       <c r="L101" s="55"/>
@@ -7332,14 +7338,14 @@
       <c r="P101" s="55"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A102" s="83"/>
-      <c r="B102" s="79"/>
-      <c r="C102" s="79"/>
+      <c r="A102" s="84"/>
+      <c r="B102" s="80"/>
+      <c r="C102" s="80"/>
       <c r="D102" s="49" t="s">
         <v>203</v>
       </c>
       <c r="H102" s="48">
-        <v>44958</v>
+        <v>44272</v>
       </c>
       <c r="K102" s="54"/>
       <c r="L102" s="55"/>
@@ -7351,13 +7357,13 @@
       <c r="P102" s="57"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A103" s="81" t="s">
+      <c r="A103" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="B103" s="77" t="s">
+      <c r="B103" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C103" s="77" t="s">
+      <c r="C103" s="78" t="s">
         <v>316</v>
       </c>
       <c r="D103" s="49" t="s">
@@ -7383,9 +7389,9 @@
       <c r="P103" s="55"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A104" s="82"/>
-      <c r="B104" s="78"/>
-      <c r="C104" s="78"/>
+      <c r="A104" s="83"/>
+      <c r="B104" s="79"/>
+      <c r="C104" s="79"/>
       <c r="D104" s="49" t="s">
         <v>197</v>
       </c>
@@ -7412,9 +7418,9 @@
       <c r="P104" s="55"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A105" s="82"/>
-      <c r="B105" s="78"/>
-      <c r="C105" s="78"/>
+      <c r="A105" s="83"/>
+      <c r="B105" s="79"/>
+      <c r="C105" s="79"/>
       <c r="D105" s="49" t="s">
         <v>197</v>
       </c>
@@ -7441,9 +7447,9 @@
       <c r="P105" s="55"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A106" s="82"/>
-      <c r="B106" s="78"/>
-      <c r="C106" s="78"/>
+      <c r="A106" s="83"/>
+      <c r="B106" s="79"/>
+      <c r="C106" s="79"/>
       <c r="D106" s="49" t="s">
         <v>200</v>
       </c>
@@ -7476,9 +7482,9 @@
       <c r="P106" s="55"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A107" s="82"/>
-      <c r="B107" s="78"/>
-      <c r="C107" s="78"/>
+      <c r="A107" s="83"/>
+      <c r="B107" s="79"/>
+      <c r="C107" s="79"/>
       <c r="D107" s="49" t="s">
         <v>200</v>
       </c>
@@ -7503,9 +7509,9 @@
       <c r="P107" s="55"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A108" s="82"/>
-      <c r="B108" s="78"/>
-      <c r="C108" s="78"/>
+      <c r="A108" s="83"/>
+      <c r="B108" s="79"/>
+      <c r="C108" s="79"/>
       <c r="D108" s="49" t="s">
         <v>200</v>
       </c>
@@ -7530,9 +7536,9 @@
       <c r="P108" s="55"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A109" s="82"/>
-      <c r="B109" s="78"/>
-      <c r="C109" s="78"/>
+      <c r="A109" s="83"/>
+      <c r="B109" s="79"/>
+      <c r="C109" s="79"/>
       <c r="D109" s="49" t="s">
         <v>202</v>
       </c>
@@ -7559,9 +7565,9 @@
       <c r="P109" s="55"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A110" s="82"/>
-      <c r="B110" s="78"/>
-      <c r="C110" s="78"/>
+      <c r="A110" s="83"/>
+      <c r="B110" s="79"/>
+      <c r="C110" s="79"/>
       <c r="D110" s="49" t="s">
         <v>202</v>
       </c>
@@ -7588,9 +7594,9 @@
       <c r="P110" s="55"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A111" s="83"/>
-      <c r="B111" s="79"/>
-      <c r="C111" s="79"/>
+      <c r="A111" s="84"/>
+      <c r="B111" s="80"/>
+      <c r="C111" s="80"/>
       <c r="D111" s="49" t="s">
         <v>203</v>
       </c>
@@ -7607,13 +7613,13 @@
       <c r="P111" s="55"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A112" s="81" t="s">
+      <c r="A112" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="B112" s="77" t="s">
+      <c r="B112" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C112" s="77" t="s">
+      <c r="C112" s="78" t="s">
         <v>316</v>
       </c>
       <c r="D112" s="49" t="s">
@@ -7639,9 +7645,9 @@
       <c r="P112" s="55"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A113" s="82"/>
-      <c r="B113" s="78"/>
-      <c r="C113" s="78"/>
+      <c r="A113" s="83"/>
+      <c r="B113" s="79"/>
+      <c r="C113" s="79"/>
       <c r="D113" s="49" t="s">
         <v>197</v>
       </c>
@@ -7668,9 +7674,9 @@
       <c r="P113" s="55"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A114" s="82"/>
-      <c r="B114" s="78"/>
-      <c r="C114" s="78"/>
+      <c r="A114" s="83"/>
+      <c r="B114" s="79"/>
+      <c r="C114" s="79"/>
       <c r="D114" s="49" t="s">
         <v>197</v>
       </c>
@@ -7697,9 +7703,9 @@
       <c r="P114" s="55"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A115" s="82"/>
-      <c r="B115" s="78"/>
-      <c r="C115" s="78"/>
+      <c r="A115" s="83"/>
+      <c r="B115" s="79"/>
+      <c r="C115" s="79"/>
       <c r="D115" s="49" t="s">
         <v>200</v>
       </c>
@@ -7732,9 +7738,9 @@
       <c r="P115" s="55"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" s="82"/>
-      <c r="B116" s="78"/>
-      <c r="C116" s="78"/>
+      <c r="A116" s="83"/>
+      <c r="B116" s="79"/>
+      <c r="C116" s="79"/>
       <c r="D116" s="49" t="s">
         <v>200</v>
       </c>
@@ -7761,9 +7767,9 @@
       <c r="P116" s="55"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A117" s="82"/>
-      <c r="B117" s="78"/>
-      <c r="C117" s="78"/>
+      <c r="A117" s="83"/>
+      <c r="B117" s="79"/>
+      <c r="C117" s="79"/>
       <c r="D117" s="49" t="s">
         <v>200</v>
       </c>
@@ -7790,9 +7796,9 @@
       <c r="P117" s="55"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" s="82"/>
-      <c r="B118" s="78"/>
-      <c r="C118" s="78"/>
+      <c r="A118" s="83"/>
+      <c r="B118" s="79"/>
+      <c r="C118" s="79"/>
       <c r="D118" s="49" t="s">
         <v>202</v>
       </c>
@@ -7819,9 +7825,9 @@
       <c r="P118" s="55"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" s="82"/>
-      <c r="B119" s="78"/>
-      <c r="C119" s="78"/>
+      <c r="A119" s="83"/>
+      <c r="B119" s="79"/>
+      <c r="C119" s="79"/>
       <c r="D119" s="49" t="s">
         <v>202</v>
       </c>
@@ -7848,9 +7854,9 @@
       <c r="P119" s="55"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A120" s="83"/>
-      <c r="B120" s="79"/>
-      <c r="C120" s="79"/>
+      <c r="A120" s="84"/>
+      <c r="B120" s="80"/>
+      <c r="C120" s="80"/>
       <c r="D120" s="49" t="s">
         <v>203</v>
       </c>
@@ -7867,13 +7873,13 @@
       <c r="P120" s="55"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A121" s="81" t="s">
+      <c r="A121" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="B121" s="77" t="s">
+      <c r="B121" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C121" s="77" t="s">
+      <c r="C121" s="78" t="s">
         <v>316</v>
       </c>
       <c r="D121" s="49" t="s">
@@ -7899,9 +7905,9 @@
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A122" s="82"/>
-      <c r="B122" s="78"/>
-      <c r="C122" s="78"/>
+      <c r="A122" s="83"/>
+      <c r="B122" s="79"/>
+      <c r="C122" s="79"/>
       <c r="D122" s="49" t="s">
         <v>197</v>
       </c>
@@ -7928,9 +7934,9 @@
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A123" s="82"/>
-      <c r="B123" s="78"/>
-      <c r="C123" s="78"/>
+      <c r="A123" s="83"/>
+      <c r="B123" s="79"/>
+      <c r="C123" s="79"/>
       <c r="D123" s="49" t="s">
         <v>197</v>
       </c>
@@ -7957,9 +7963,9 @@
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A124" s="82"/>
-      <c r="B124" s="78"/>
-      <c r="C124" s="78"/>
+      <c r="A124" s="83"/>
+      <c r="B124" s="79"/>
+      <c r="C124" s="79"/>
       <c r="D124" s="49" t="s">
         <v>200</v>
       </c>
@@ -7992,9 +7998,9 @@
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A125" s="82"/>
-      <c r="B125" s="78"/>
-      <c r="C125" s="78"/>
+      <c r="A125" s="83"/>
+      <c r="B125" s="79"/>
+      <c r="C125" s="79"/>
       <c r="D125" s="49" t="s">
         <v>200</v>
       </c>
@@ -8021,9 +8027,9 @@
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A126" s="82"/>
-      <c r="B126" s="78"/>
-      <c r="C126" s="78"/>
+      <c r="A126" s="83"/>
+      <c r="B126" s="79"/>
+      <c r="C126" s="79"/>
       <c r="D126" s="49" t="s">
         <v>200</v>
       </c>
@@ -8050,9 +8056,9 @@
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A127" s="82"/>
-      <c r="B127" s="78"/>
-      <c r="C127" s="78"/>
+      <c r="A127" s="83"/>
+      <c r="B127" s="79"/>
+      <c r="C127" s="79"/>
       <c r="D127" s="49" t="s">
         <v>202</v>
       </c>
@@ -8079,9 +8085,9 @@
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A128" s="82"/>
-      <c r="B128" s="78"/>
-      <c r="C128" s="78"/>
+      <c r="A128" s="83"/>
+      <c r="B128" s="79"/>
+      <c r="C128" s="79"/>
       <c r="D128" s="49" t="s">
         <v>202</v>
       </c>
@@ -8108,9 +8114,9 @@
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A129" s="83"/>
-      <c r="B129" s="79"/>
-      <c r="C129" s="79"/>
+      <c r="A129" s="84"/>
+      <c r="B129" s="80"/>
+      <c r="C129" s="80"/>
       <c r="D129" s="49" t="s">
         <v>203</v>
       </c>
@@ -8127,13 +8133,13 @@
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A130" s="81" t="s">
+      <c r="A130" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="B130" s="77" t="s">
+      <c r="B130" s="78" t="s">
         <v>315</v>
       </c>
-      <c r="C130" s="77" t="s">
+      <c r="C130" s="78" t="s">
         <v>316</v>
       </c>
       <c r="D130" s="49" t="s">
@@ -8160,9 +8166,9 @@
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A131" s="82"/>
-      <c r="B131" s="78"/>
-      <c r="C131" s="78"/>
+      <c r="A131" s="83"/>
+      <c r="B131" s="79"/>
+      <c r="C131" s="79"/>
       <c r="D131" s="49" t="s">
         <v>196</v>
       </c>
@@ -8190,9 +8196,9 @@
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A132" s="82"/>
-      <c r="B132" s="78"/>
-      <c r="C132" s="78"/>
+      <c r="A132" s="83"/>
+      <c r="B132" s="79"/>
+      <c r="C132" s="79"/>
       <c r="D132" s="49" t="s">
         <v>197</v>
       </c>
@@ -8220,9 +8226,9 @@
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A133" s="82"/>
-      <c r="B133" s="78"/>
-      <c r="C133" s="78"/>
+      <c r="A133" s="83"/>
+      <c r="B133" s="79"/>
+      <c r="C133" s="79"/>
       <c r="D133" s="49" t="s">
         <v>197</v>
       </c>
@@ -8250,9 +8256,9 @@
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A134" s="82"/>
-      <c r="B134" s="78"/>
-      <c r="C134" s="78"/>
+      <c r="A134" s="83"/>
+      <c r="B134" s="79"/>
+      <c r="C134" s="79"/>
       <c r="D134" s="49" t="s">
         <v>200</v>
       </c>
@@ -8286,9 +8292,9 @@
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A135" s="82"/>
-      <c r="B135" s="78"/>
-      <c r="C135" s="78"/>
+      <c r="A135" s="83"/>
+      <c r="B135" s="79"/>
+      <c r="C135" s="79"/>
       <c r="D135" s="49" t="s">
         <v>200</v>
       </c>
@@ -8316,9 +8322,9 @@
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A136" s="82"/>
-      <c r="B136" s="78"/>
-      <c r="C136" s="78"/>
+      <c r="A136" s="83"/>
+      <c r="B136" s="79"/>
+      <c r="C136" s="79"/>
       <c r="D136" s="49" t="s">
         <v>200</v>
       </c>
@@ -8346,9 +8352,9 @@
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A137" s="82"/>
-      <c r="B137" s="78"/>
-      <c r="C137" s="78"/>
+      <c r="A137" s="83"/>
+      <c r="B137" s="79"/>
+      <c r="C137" s="79"/>
       <c r="D137" s="49" t="s">
         <v>202</v>
       </c>
@@ -8376,9 +8382,9 @@
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A138" s="82"/>
-      <c r="B138" s="78"/>
-      <c r="C138" s="78"/>
+      <c r="A138" s="83"/>
+      <c r="B138" s="79"/>
+      <c r="C138" s="79"/>
       <c r="D138" s="49" t="s">
         <v>202</v>
       </c>
@@ -8406,9 +8412,9 @@
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A139" s="83"/>
-      <c r="B139" s="79"/>
-      <c r="C139" s="79"/>
+      <c r="A139" s="84"/>
+      <c r="B139" s="80"/>
+      <c r="C139" s="80"/>
       <c r="D139" s="49" t="s">
         <v>203</v>
       </c>
@@ -8426,13 +8432,13 @@
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A140" s="76" t="s">
+      <c r="A140" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B140" s="77" t="s">
+      <c r="B140" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C140" s="80" t="s">
+      <c r="C140" s="81" t="s">
         <v>78</v>
       </c>
       <c r="D140" s="49" t="s">
@@ -8462,9 +8468,9 @@
       <c r="P140" s="55"/>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A141" s="76"/>
-      <c r="B141" s="78"/>
-      <c r="C141" s="80"/>
+      <c r="A141" s="77"/>
+      <c r="B141" s="79"/>
+      <c r="C141" s="81"/>
       <c r="D141" s="49" t="s">
         <v>197</v>
       </c>
@@ -8495,9 +8501,9 @@
       <c r="P141" s="55"/>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A142" s="76"/>
-      <c r="B142" s="78"/>
-      <c r="C142" s="80"/>
+      <c r="A142" s="77"/>
+      <c r="B142" s="79"/>
+      <c r="C142" s="81"/>
       <c r="D142" s="49" t="s">
         <v>199</v>
       </c>
@@ -8528,9 +8534,9 @@
       <c r="P142" s="55"/>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A143" s="76"/>
-      <c r="B143" s="78"/>
-      <c r="C143" s="80"/>
+      <c r="A143" s="77"/>
+      <c r="B143" s="79"/>
+      <c r="C143" s="81"/>
       <c r="D143" s="49" t="s">
         <v>200</v>
       </c>
@@ -8551,9 +8557,9 @@
       <c r="P143" s="55"/>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A144" s="76"/>
-      <c r="B144" s="78"/>
-      <c r="C144" s="80"/>
+      <c r="A144" s="77"/>
+      <c r="B144" s="79"/>
+      <c r="C144" s="81"/>
       <c r="D144" s="49" t="s">
         <v>202</v>
       </c>
@@ -8581,9 +8587,9 @@
       <c r="P144" s="55"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A145" s="76"/>
-      <c r="B145" s="79"/>
-      <c r="C145" s="80"/>
+      <c r="A145" s="77"/>
+      <c r="B145" s="80"/>
+      <c r="C145" s="81"/>
       <c r="D145" s="49" t="s">
         <v>203</v>
       </c>
@@ -8596,13 +8602,13 @@
       <c r="P145" s="55"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A146" s="76" t="s">
+      <c r="A146" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B146" s="77" t="s">
+      <c r="B146" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C146" s="80" t="s">
+      <c r="C146" s="81" t="s">
         <v>78</v>
       </c>
       <c r="D146" s="49" t="s">
@@ -8622,9 +8628,9 @@
       <c r="P146" s="55"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A147" s="76"/>
-      <c r="B147" s="78"/>
-      <c r="C147" s="80"/>
+      <c r="A147" s="77"/>
+      <c r="B147" s="79"/>
+      <c r="C147" s="81"/>
       <c r="D147" s="49" t="s">
         <v>196</v>
       </c>
@@ -8658,9 +8664,9 @@
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A148" s="76"/>
-      <c r="B148" s="78"/>
-      <c r="C148" s="80"/>
+      <c r="A148" s="77"/>
+      <c r="B148" s="79"/>
+      <c r="C148" s="81"/>
       <c r="D148" s="49" t="s">
         <v>196</v>
       </c>
@@ -8694,9 +8700,9 @@
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A149" s="76"/>
-      <c r="B149" s="78"/>
-      <c r="C149" s="80"/>
+      <c r="A149" s="77"/>
+      <c r="B149" s="79"/>
+      <c r="C149" s="81"/>
       <c r="D149" s="49" t="s">
         <v>196</v>
       </c>
@@ -8730,9 +8736,9 @@
       </c>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A150" s="76"/>
-      <c r="B150" s="78"/>
-      <c r="C150" s="80"/>
+      <c r="A150" s="77"/>
+      <c r="B150" s="79"/>
+      <c r="C150" s="81"/>
       <c r="D150" s="49" t="s">
         <v>196</v>
       </c>
@@ -8766,9 +8772,9 @@
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A151" s="76"/>
-      <c r="B151" s="78"/>
-      <c r="C151" s="80"/>
+      <c r="A151" s="77"/>
+      <c r="B151" s="79"/>
+      <c r="C151" s="81"/>
       <c r="D151" s="49" t="s">
         <v>196</v>
       </c>
@@ -8802,9 +8808,9 @@
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A152" s="76"/>
-      <c r="B152" s="78"/>
-      <c r="C152" s="80"/>
+      <c r="A152" s="77"/>
+      <c r="B152" s="79"/>
+      <c r="C152" s="81"/>
       <c r="D152" s="49" t="s">
         <v>197</v>
       </c>
@@ -8838,9 +8844,9 @@
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A153" s="76"/>
-      <c r="B153" s="78"/>
-      <c r="C153" s="80"/>
+      <c r="A153" s="77"/>
+      <c r="B153" s="79"/>
+      <c r="C153" s="81"/>
       <c r="D153" s="49" t="s">
         <v>197</v>
       </c>
@@ -8874,9 +8880,9 @@
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A154" s="76"/>
-      <c r="B154" s="78"/>
-      <c r="C154" s="80"/>
+      <c r="A154" s="77"/>
+      <c r="B154" s="79"/>
+      <c r="C154" s="81"/>
       <c r="D154" s="49" t="s">
         <v>293</v>
       </c>
@@ -8913,9 +8919,9 @@
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A155" s="76"/>
-      <c r="B155" s="78"/>
-      <c r="C155" s="80"/>
+      <c r="A155" s="77"/>
+      <c r="B155" s="79"/>
+      <c r="C155" s="81"/>
       <c r="D155" s="49" t="s">
         <v>196</v>
       </c>
@@ -8946,9 +8952,9 @@
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A156" s="76"/>
-      <c r="B156" s="78"/>
-      <c r="C156" s="80"/>
+      <c r="A156" s="77"/>
+      <c r="B156" s="79"/>
+      <c r="C156" s="81"/>
       <c r="D156" s="49" t="s">
         <v>293</v>
       </c>
@@ -8985,9 +8991,9 @@
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A157" s="76"/>
-      <c r="B157" s="78"/>
-      <c r="C157" s="80"/>
+      <c r="A157" s="77"/>
+      <c r="B157" s="79"/>
+      <c r="C157" s="81"/>
       <c r="D157" s="49" t="s">
         <v>294</v>
       </c>
@@ -9021,9 +9027,9 @@
       </c>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A158" s="76"/>
-      <c r="B158" s="78"/>
-      <c r="C158" s="80"/>
+      <c r="A158" s="77"/>
+      <c r="B158" s="79"/>
+      <c r="C158" s="81"/>
       <c r="D158" s="49" t="s">
         <v>200</v>
       </c>
@@ -9050,9 +9056,9 @@
       </c>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A159" s="76"/>
-      <c r="B159" s="78"/>
-      <c r="C159" s="80"/>
+      <c r="A159" s="77"/>
+      <c r="B159" s="79"/>
+      <c r="C159" s="81"/>
       <c r="D159" s="49" t="s">
         <v>200</v>
       </c>
@@ -9079,9 +9085,9 @@
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A160" s="76"/>
-      <c r="B160" s="78"/>
-      <c r="C160" s="80"/>
+      <c r="A160" s="77"/>
+      <c r="B160" s="79"/>
+      <c r="C160" s="81"/>
       <c r="D160" s="49" t="s">
         <v>202</v>
       </c>
@@ -9118,9 +9124,9 @@
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A161" s="76"/>
-      <c r="B161" s="78"/>
-      <c r="C161" s="80"/>
+      <c r="A161" s="77"/>
+      <c r="B161" s="79"/>
+      <c r="C161" s="81"/>
       <c r="D161" s="49" t="s">
         <v>266</v>
       </c>
@@ -9157,9 +9163,9 @@
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A162" s="76"/>
-      <c r="B162" s="78"/>
-      <c r="C162" s="80"/>
+      <c r="A162" s="77"/>
+      <c r="B162" s="79"/>
+      <c r="C162" s="81"/>
       <c r="D162" s="49" t="s">
         <v>266</v>
       </c>
@@ -9196,9 +9202,9 @@
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A163" s="76"/>
-      <c r="B163" s="78"/>
-      <c r="C163" s="80"/>
+      <c r="A163" s="77"/>
+      <c r="B163" s="79"/>
+      <c r="C163" s="81"/>
       <c r="D163" s="49" t="s">
         <v>261</v>
       </c>
@@ -9229,9 +9235,9 @@
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A164" s="76"/>
-      <c r="B164" s="79"/>
-      <c r="C164" s="80"/>
+      <c r="A164" s="77"/>
+      <c r="B164" s="80"/>
+      <c r="C164" s="81"/>
       <c r="D164" s="49" t="s">
         <v>203</v>
       </c>
@@ -9246,13 +9252,13 @@
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A165" s="76" t="s">
+      <c r="A165" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="B165" s="77" t="s">
+      <c r="B165" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="C165" s="80" t="s">
+      <c r="C165" s="81" t="s">
         <v>242</v>
       </c>
       <c r="D165" s="49" t="s">
@@ -9276,9 +9282,9 @@
       <c r="P165" s="55"/>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A166" s="76"/>
-      <c r="B166" s="78"/>
-      <c r="C166" s="80"/>
+      <c r="A166" s="77"/>
+      <c r="B166" s="79"/>
+      <c r="C166" s="81"/>
       <c r="D166" s="49" t="s">
         <v>197</v>
       </c>
@@ -9303,9 +9309,9 @@
       <c r="P166" s="55"/>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A167" s="76"/>
-      <c r="B167" s="78"/>
-      <c r="C167" s="80"/>
+      <c r="A167" s="77"/>
+      <c r="B167" s="79"/>
+      <c r="C167" s="81"/>
       <c r="D167" s="49" t="s">
         <v>267</v>
       </c>
@@ -9330,9 +9336,9 @@
       <c r="P167" s="55"/>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A168" s="76"/>
-      <c r="B168" s="78"/>
-      <c r="C168" s="80"/>
+      <c r="A168" s="77"/>
+      <c r="B168" s="79"/>
+      <c r="C168" s="81"/>
       <c r="D168" s="49" t="s">
         <v>200</v>
       </c>
@@ -9355,9 +9361,9 @@
       <c r="P168" s="55"/>
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A169" s="76"/>
-      <c r="B169" s="78"/>
-      <c r="C169" s="80"/>
+      <c r="A169" s="77"/>
+      <c r="B169" s="79"/>
+      <c r="C169" s="81"/>
       <c r="D169" s="49" t="s">
         <v>200</v>
       </c>
@@ -9380,9 +9386,9 @@
       <c r="P169" s="55"/>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A170" s="76"/>
-      <c r="B170" s="78"/>
-      <c r="C170" s="80"/>
+      <c r="A170" s="77"/>
+      <c r="B170" s="79"/>
+      <c r="C170" s="81"/>
       <c r="D170" s="49" t="s">
         <v>200</v>
       </c>
@@ -9405,9 +9411,9 @@
       <c r="P170" s="55"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A171" s="76"/>
-      <c r="B171" s="78"/>
-      <c r="C171" s="80"/>
+      <c r="A171" s="77"/>
+      <c r="B171" s="79"/>
+      <c r="C171" s="81"/>
       <c r="D171" s="49" t="s">
         <v>200</v>
       </c>
@@ -9430,9 +9436,9 @@
       <c r="P171" s="55"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A172" s="76"/>
-      <c r="B172" s="78"/>
-      <c r="C172" s="80"/>
+      <c r="A172" s="77"/>
+      <c r="B172" s="79"/>
+      <c r="C172" s="81"/>
       <c r="D172" s="49" t="s">
         <v>200</v>
       </c>
@@ -9455,9 +9461,9 @@
       <c r="P172" s="55"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A173" s="76"/>
-      <c r="B173" s="78"/>
-      <c r="C173" s="80"/>
+      <c r="A173" s="77"/>
+      <c r="B173" s="79"/>
+      <c r="C173" s="81"/>
       <c r="D173" s="49" t="s">
         <v>200</v>
       </c>
@@ -9480,9 +9486,9 @@
       <c r="P173" s="55"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A174" s="76"/>
-      <c r="B174" s="78"/>
-      <c r="C174" s="80"/>
+      <c r="A174" s="77"/>
+      <c r="B174" s="79"/>
+      <c r="C174" s="81"/>
       <c r="D174" s="49" t="s">
         <v>200</v>
       </c>
@@ -9505,9 +9511,9 @@
       <c r="P174" s="55"/>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A175" s="76"/>
-      <c r="B175" s="78"/>
-      <c r="C175" s="80"/>
+      <c r="A175" s="77"/>
+      <c r="B175" s="79"/>
+      <c r="C175" s="81"/>
       <c r="D175" s="49" t="s">
         <v>200</v>
       </c>
@@ -9530,9 +9536,9 @@
       <c r="P175" s="55"/>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A176" s="76"/>
-      <c r="B176" s="78"/>
-      <c r="C176" s="80"/>
+      <c r="A176" s="77"/>
+      <c r="B176" s="79"/>
+      <c r="C176" s="81"/>
       <c r="D176" s="49" t="s">
         <v>200</v>
       </c>
@@ -9555,9 +9561,9 @@
       <c r="P176" s="55"/>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A177" s="76"/>
-      <c r="B177" s="78"/>
-      <c r="C177" s="80"/>
+      <c r="A177" s="77"/>
+      <c r="B177" s="79"/>
+      <c r="C177" s="81"/>
       <c r="D177" s="49" t="s">
         <v>200</v>
       </c>
@@ -9580,9 +9586,9 @@
       <c r="P177" s="55"/>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A178" s="76"/>
-      <c r="B178" s="78"/>
-      <c r="C178" s="80"/>
+      <c r="A178" s="77"/>
+      <c r="B178" s="79"/>
+      <c r="C178" s="81"/>
       <c r="D178" s="49" t="s">
         <v>200</v>
       </c>
@@ -9607,9 +9613,9 @@
       <c r="P178" s="55"/>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A179" s="76"/>
-      <c r="B179" s="78"/>
-      <c r="C179" s="80"/>
+      <c r="A179" s="77"/>
+      <c r="B179" s="79"/>
+      <c r="C179" s="81"/>
       <c r="D179" s="49" t="s">
         <v>202</v>
       </c>
@@ -9632,9 +9638,9 @@
       <c r="P179" s="55"/>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A180" s="76"/>
-      <c r="B180" s="79"/>
-      <c r="C180" s="80"/>
+      <c r="A180" s="77"/>
+      <c r="B180" s="80"/>
+      <c r="C180" s="81"/>
       <c r="D180" s="49" t="s">
         <v>203</v>
       </c>
@@ -9651,13 +9657,13 @@
       <c r="P180" s="55"/>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A181" s="76" t="s">
+      <c r="A181" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="B181" s="77" t="s">
+      <c r="B181" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="C181" s="80" t="s">
+      <c r="C181" s="81" t="s">
         <v>242</v>
       </c>
       <c r="D181" s="49" t="s">
@@ -9683,9 +9689,9 @@
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A182" s="76"/>
-      <c r="B182" s="78"/>
-      <c r="C182" s="80"/>
+      <c r="A182" s="77"/>
+      <c r="B182" s="79"/>
+      <c r="C182" s="81"/>
       <c r="D182" s="49" t="s">
         <v>197</v>
       </c>
@@ -9712,9 +9718,9 @@
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A183" s="76"/>
-      <c r="B183" s="78"/>
-      <c r="C183" s="80"/>
+      <c r="A183" s="77"/>
+      <c r="B183" s="79"/>
+      <c r="C183" s="81"/>
       <c r="D183" s="49" t="s">
         <v>267</v>
       </c>
@@ -9741,9 +9747,9 @@
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A184" s="76"/>
-      <c r="B184" s="78"/>
-      <c r="C184" s="80"/>
+      <c r="A184" s="77"/>
+      <c r="B184" s="79"/>
+      <c r="C184" s="81"/>
       <c r="D184" s="49" t="s">
         <v>200</v>
       </c>
@@ -9770,9 +9776,9 @@
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A185" s="76"/>
-      <c r="B185" s="78"/>
-      <c r="C185" s="80"/>
+      <c r="A185" s="77"/>
+      <c r="B185" s="79"/>
+      <c r="C185" s="81"/>
       <c r="D185" s="49" t="s">
         <v>200</v>
       </c>
@@ -9799,9 +9805,9 @@
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A186" s="76"/>
-      <c r="B186" s="78"/>
-      <c r="C186" s="80"/>
+      <c r="A186" s="77"/>
+      <c r="B186" s="79"/>
+      <c r="C186" s="81"/>
       <c r="D186" s="49" t="s">
         <v>200</v>
       </c>
@@ -9828,9 +9834,9 @@
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A187" s="76"/>
-      <c r="B187" s="78"/>
-      <c r="C187" s="80"/>
+      <c r="A187" s="77"/>
+      <c r="B187" s="79"/>
+      <c r="C187" s="81"/>
       <c r="D187" s="49" t="s">
         <v>200</v>
       </c>
@@ -9857,9 +9863,9 @@
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A188" s="76"/>
-      <c r="B188" s="78"/>
-      <c r="C188" s="80"/>
+      <c r="A188" s="77"/>
+      <c r="B188" s="79"/>
+      <c r="C188" s="81"/>
       <c r="D188" s="49" t="s">
         <v>200</v>
       </c>
@@ -9886,9 +9892,9 @@
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A189" s="76"/>
-      <c r="B189" s="78"/>
-      <c r="C189" s="80"/>
+      <c r="A189" s="77"/>
+      <c r="B189" s="79"/>
+      <c r="C189" s="81"/>
       <c r="D189" s="49" t="s">
         <v>200</v>
       </c>
@@ -9915,9 +9921,9 @@
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A190" s="76"/>
-      <c r="B190" s="78"/>
-      <c r="C190" s="80"/>
+      <c r="A190" s="77"/>
+      <c r="B190" s="79"/>
+      <c r="C190" s="81"/>
       <c r="D190" s="49" t="s">
         <v>200</v>
       </c>
@@ -9944,9 +9950,9 @@
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A191" s="76"/>
-      <c r="B191" s="78"/>
-      <c r="C191" s="80"/>
+      <c r="A191" s="77"/>
+      <c r="B191" s="79"/>
+      <c r="C191" s="81"/>
       <c r="D191" s="49" t="s">
         <v>200</v>
       </c>
@@ -9973,9 +9979,9 @@
       </c>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A192" s="76"/>
-      <c r="B192" s="78"/>
-      <c r="C192" s="80"/>
+      <c r="A192" s="77"/>
+      <c r="B192" s="79"/>
+      <c r="C192" s="81"/>
       <c r="D192" s="49" t="s">
         <v>200</v>
       </c>
@@ -10002,9 +10008,9 @@
       </c>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A193" s="76"/>
-      <c r="B193" s="78"/>
-      <c r="C193" s="80"/>
+      <c r="A193" s="77"/>
+      <c r="B193" s="79"/>
+      <c r="C193" s="81"/>
       <c r="D193" s="49" t="s">
         <v>200</v>
       </c>
@@ -10031,9 +10037,9 @@
       </c>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A194" s="76"/>
-      <c r="B194" s="78"/>
-      <c r="C194" s="80"/>
+      <c r="A194" s="77"/>
+      <c r="B194" s="79"/>
+      <c r="C194" s="81"/>
       <c r="D194" s="49" t="s">
         <v>200</v>
       </c>
@@ -10060,9 +10066,9 @@
       </c>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A195" s="76"/>
-      <c r="B195" s="78"/>
-      <c r="C195" s="80"/>
+      <c r="A195" s="77"/>
+      <c r="B195" s="79"/>
+      <c r="C195" s="81"/>
       <c r="D195" s="49" t="s">
         <v>202</v>
       </c>
@@ -10087,9 +10093,9 @@
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A196" s="76"/>
-      <c r="B196" s="79"/>
-      <c r="C196" s="80"/>
+      <c r="A196" s="77"/>
+      <c r="B196" s="80"/>
+      <c r="C196" s="81"/>
       <c r="D196" s="49" t="s">
         <v>203</v>
       </c>
@@ -10106,13 +10112,13 @@
       </c>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A197" s="76" t="s">
+      <c r="A197" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="B197" s="77" t="s">
+      <c r="B197" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="C197" s="80" t="s">
+      <c r="C197" s="81" t="s">
         <v>81</v>
       </c>
       <c r="D197" s="49" t="s">
@@ -10145,9 +10151,9 @@
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A198" s="76"/>
-      <c r="B198" s="78"/>
-      <c r="C198" s="80"/>
+      <c r="A198" s="77"/>
+      <c r="B198" s="79"/>
+      <c r="C198" s="81"/>
       <c r="D198" s="49" t="s">
         <v>257</v>
       </c>
@@ -10178,9 +10184,9 @@
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A199" s="76"/>
-      <c r="B199" s="78"/>
-      <c r="C199" s="80"/>
+      <c r="A199" s="77"/>
+      <c r="B199" s="79"/>
+      <c r="C199" s="81"/>
       <c r="D199" s="49" t="s">
         <v>197</v>
       </c>
@@ -10207,9 +10213,9 @@
       </c>
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A200" s="76"/>
-      <c r="B200" s="78"/>
-      <c r="C200" s="80"/>
+      <c r="A200" s="77"/>
+      <c r="B200" s="79"/>
+      <c r="C200" s="81"/>
       <c r="D200" s="49" t="s">
         <v>199</v>
       </c>
@@ -10245,9 +10251,9 @@
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A201" s="76"/>
-      <c r="B201" s="78"/>
-      <c r="C201" s="80"/>
+      <c r="A201" s="77"/>
+      <c r="B201" s="79"/>
+      <c r="C201" s="81"/>
       <c r="D201" s="49" t="s">
         <v>200</v>
       </c>
@@ -10278,9 +10284,9 @@
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A202" s="76"/>
-      <c r="B202" s="78"/>
-      <c r="C202" s="80"/>
+      <c r="A202" s="77"/>
+      <c r="B202" s="79"/>
+      <c r="C202" s="81"/>
       <c r="D202" s="49" t="s">
         <v>202</v>
       </c>
@@ -10313,9 +10319,9 @@
       </c>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A203" s="76"/>
-      <c r="B203" s="78"/>
-      <c r="C203" s="80"/>
+      <c r="A203" s="77"/>
+      <c r="B203" s="79"/>
+      <c r="C203" s="81"/>
       <c r="D203" s="49" t="s">
         <v>227</v>
       </c>
@@ -10330,9 +10336,9 @@
       </c>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A204" s="76"/>
-      <c r="B204" s="79"/>
-      <c r="C204" s="80"/>
+      <c r="A204" s="77"/>
+      <c r="B204" s="80"/>
+      <c r="C204" s="81"/>
       <c r="D204" s="49" t="s">
         <v>203</v>
       </c>
@@ -10347,13 +10353,13 @@
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A205" s="76" t="s">
+      <c r="A205" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B205" s="77" t="s">
+      <c r="B205" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="C205" s="80" t="s">
+      <c r="C205" s="81" t="s">
         <v>84</v>
       </c>
       <c r="D205" s="49" t="s">
@@ -10383,9 +10389,9 @@
       <c r="P205" s="55"/>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A206" s="76"/>
-      <c r="B206" s="78"/>
-      <c r="C206" s="80"/>
+      <c r="A206" s="77"/>
+      <c r="B206" s="79"/>
+      <c r="C206" s="81"/>
       <c r="D206" s="49" t="s">
         <v>197</v>
       </c>
@@ -10416,9 +10422,9 @@
       <c r="P206" s="55"/>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A207" s="76"/>
-      <c r="B207" s="78"/>
-      <c r="C207" s="80"/>
+      <c r="A207" s="77"/>
+      <c r="B207" s="79"/>
+      <c r="C207" s="81"/>
       <c r="D207" s="49" t="s">
         <v>199</v>
       </c>
@@ -10449,9 +10455,9 @@
       <c r="P207" s="55"/>
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A208" s="76"/>
-      <c r="B208" s="78"/>
-      <c r="C208" s="80"/>
+      <c r="A208" s="77"/>
+      <c r="B208" s="79"/>
+      <c r="C208" s="81"/>
       <c r="D208" s="49" t="s">
         <v>200</v>
       </c>
@@ -10472,9 +10478,9 @@
       <c r="P208" s="55"/>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A209" s="76"/>
-      <c r="B209" s="78"/>
-      <c r="C209" s="80"/>
+      <c r="A209" s="77"/>
+      <c r="B209" s="79"/>
+      <c r="C209" s="81"/>
       <c r="D209" s="49" t="s">
         <v>202</v>
       </c>
@@ -10502,9 +10508,9 @@
       <c r="P209" s="55"/>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A210" s="76"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="80"/>
+      <c r="A210" s="77"/>
+      <c r="B210" s="80"/>
+      <c r="C210" s="81"/>
       <c r="D210" s="49" t="s">
         <v>203</v>
       </c>
@@ -10517,13 +10523,13 @@
       <c r="P210" s="55"/>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A211" s="76" t="s">
+      <c r="A211" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B211" s="77" t="s">
+      <c r="B211" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="C211" s="80" t="s">
+      <c r="C211" s="81" t="s">
         <v>84</v>
       </c>
       <c r="D211" s="49" t="s">
@@ -10549,9 +10555,9 @@
       </c>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A212" s="76"/>
-      <c r="B212" s="78"/>
-      <c r="C212" s="80"/>
+      <c r="A212" s="77"/>
+      <c r="B212" s="79"/>
+      <c r="C212" s="81"/>
       <c r="D212" s="49" t="s">
         <v>197</v>
       </c>
@@ -10578,9 +10584,9 @@
       </c>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A213" s="76"/>
-      <c r="B213" s="78"/>
-      <c r="C213" s="80"/>
+      <c r="A213" s="77"/>
+      <c r="B213" s="79"/>
+      <c r="C213" s="81"/>
       <c r="D213" s="49" t="s">
         <v>285</v>
       </c>
@@ -10610,9 +10616,9 @@
       </c>
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A214" s="76"/>
-      <c r="B214" s="78"/>
-      <c r="C214" s="80"/>
+      <c r="A214" s="77"/>
+      <c r="B214" s="79"/>
+      <c r="C214" s="81"/>
       <c r="D214" s="49" t="s">
         <v>307</v>
       </c>
@@ -10636,9 +10642,9 @@
       </c>
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A215" s="76"/>
-      <c r="B215" s="78"/>
-      <c r="C215" s="80"/>
+      <c r="A215" s="77"/>
+      <c r="B215" s="79"/>
+      <c r="C215" s="81"/>
       <c r="D215" s="49" t="s">
         <v>200</v>
       </c>
@@ -10666,9 +10672,9 @@
       </c>
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A216" s="76"/>
-      <c r="B216" s="78"/>
-      <c r="C216" s="80"/>
+      <c r="A216" s="77"/>
+      <c r="B216" s="79"/>
+      <c r="C216" s="81"/>
       <c r="D216" s="49" t="s">
         <v>202</v>
       </c>
@@ -10695,9 +10701,9 @@
       </c>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A217" s="76"/>
-      <c r="B217" s="79"/>
-      <c r="C217" s="80"/>
+      <c r="A217" s="77"/>
+      <c r="B217" s="80"/>
+      <c r="C217" s="81"/>
       <c r="D217" s="49" t="s">
         <v>203</v>
       </c>
@@ -10712,13 +10718,13 @@
       </c>
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A218" s="76" t="s">
+      <c r="A218" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="B218" s="77" t="s">
+      <c r="B218" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="C218" s="80" t="s">
+      <c r="C218" s="81" t="s">
         <v>87</v>
       </c>
       <c r="D218" s="49" t="s">
@@ -10754,9 +10760,9 @@
       </c>
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A219" s="76"/>
-      <c r="B219" s="78"/>
-      <c r="C219" s="80"/>
+      <c r="A219" s="77"/>
+      <c r="B219" s="79"/>
+      <c r="C219" s="81"/>
       <c r="D219" s="49" t="s">
         <v>196</v>
       </c>
@@ -10790,9 +10796,9 @@
       </c>
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A220" s="76"/>
-      <c r="B220" s="78"/>
-      <c r="C220" s="80"/>
+      <c r="A220" s="77"/>
+      <c r="B220" s="79"/>
+      <c r="C220" s="81"/>
       <c r="D220" s="49" t="s">
         <v>196</v>
       </c>
@@ -10826,9 +10832,9 @@
       </c>
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A221" s="76"/>
-      <c r="B221" s="78"/>
-      <c r="C221" s="80"/>
+      <c r="A221" s="77"/>
+      <c r="B221" s="79"/>
+      <c r="C221" s="81"/>
       <c r="D221" s="49" t="s">
         <v>197</v>
       </c>
@@ -10862,9 +10868,9 @@
       </c>
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A222" s="76"/>
-      <c r="B222" s="78"/>
-      <c r="C222" s="80"/>
+      <c r="A222" s="77"/>
+      <c r="B222" s="79"/>
+      <c r="C222" s="81"/>
       <c r="D222" s="49" t="s">
         <v>197</v>
       </c>
@@ -10898,9 +10904,9 @@
       </c>
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A223" s="76"/>
-      <c r="B223" s="78"/>
-      <c r="C223" s="80"/>
+      <c r="A223" s="77"/>
+      <c r="B223" s="79"/>
+      <c r="C223" s="81"/>
       <c r="D223" s="49" t="s">
         <v>197</v>
       </c>
@@ -10932,9 +10938,9 @@
       </c>
     </row>
     <row r="224" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="76"/>
-      <c r="B224" s="78"/>
-      <c r="C224" s="80"/>
+      <c r="A224" s="77"/>
+      <c r="B224" s="79"/>
+      <c r="C224" s="81"/>
       <c r="D224" s="58" t="s">
         <v>285</v>
       </c>
@@ -10975,9 +10981,9 @@
       <c r="Q224" s="54"/>
     </row>
     <row r="225" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="76"/>
-      <c r="B225" s="78"/>
-      <c r="C225" s="80"/>
+      <c r="A225" s="77"/>
+      <c r="B225" s="79"/>
+      <c r="C225" s="81"/>
       <c r="D225" s="58" t="s">
         <v>285</v>
       </c>
@@ -11018,9 +11024,9 @@
       <c r="Q225" s="54"/>
     </row>
     <row r="226" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="76"/>
-      <c r="B226" s="78"/>
-      <c r="C226" s="80"/>
+      <c r="A226" s="77"/>
+      <c r="B226" s="79"/>
+      <c r="C226" s="81"/>
       <c r="D226" s="58" t="s">
         <v>285</v>
       </c>
@@ -11058,9 +11064,9 @@
       <c r="Q226" s="54"/>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A227" s="76"/>
-      <c r="B227" s="78"/>
-      <c r="C227" s="80"/>
+      <c r="A227" s="77"/>
+      <c r="B227" s="79"/>
+      <c r="C227" s="81"/>
       <c r="D227" s="49" t="s">
         <v>200</v>
       </c>
@@ -11092,9 +11098,9 @@
       </c>
     </row>
     <row r="228" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="76"/>
-      <c r="B228" s="78"/>
-      <c r="C228" s="80"/>
+      <c r="A228" s="77"/>
+      <c r="B228" s="79"/>
+      <c r="C228" s="81"/>
       <c r="D228" s="58" t="s">
         <v>200</v>
       </c>
@@ -11129,9 +11135,9 @@
       <c r="Q228" s="54"/>
     </row>
     <row r="229" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="76"/>
-      <c r="B229" s="78"/>
-      <c r="C229" s="80"/>
+      <c r="A229" s="77"/>
+      <c r="B229" s="79"/>
+      <c r="C229" s="81"/>
       <c r="D229" s="58" t="s">
         <v>200</v>
       </c>
@@ -11166,9 +11172,9 @@
       <c r="Q229" s="54"/>
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A230" s="76"/>
-      <c r="B230" s="78"/>
-      <c r="C230" s="80"/>
+      <c r="A230" s="77"/>
+      <c r="B230" s="79"/>
+      <c r="C230" s="81"/>
       <c r="D230" s="49" t="s">
         <v>202</v>
       </c>
@@ -11200,9 +11206,9 @@
       </c>
     </row>
     <row r="231" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A231" s="76"/>
-      <c r="B231" s="78"/>
-      <c r="C231" s="80"/>
+      <c r="A231" s="77"/>
+      <c r="B231" s="79"/>
+      <c r="C231" s="81"/>
       <c r="D231" s="49" t="s">
         <v>202</v>
       </c>
@@ -11232,9 +11238,9 @@
       </c>
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A232" s="76"/>
-      <c r="B232" s="78"/>
-      <c r="C232" s="80"/>
+      <c r="A232" s="77"/>
+      <c r="B232" s="79"/>
+      <c r="C232" s="81"/>
       <c r="D232" s="49" t="s">
         <v>202</v>
       </c>
@@ -11264,9 +11270,9 @@
       </c>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A233" s="76"/>
-      <c r="B233" s="79"/>
-      <c r="C233" s="80"/>
+      <c r="A233" s="77"/>
+      <c r="B233" s="80"/>
+      <c r="C233" s="81"/>
       <c r="D233" s="49" t="s">
         <v>203</v>
       </c>
@@ -11281,13 +11287,13 @@
       </c>
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A234" s="76" t="s">
+      <c r="A234" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="B234" s="77" t="s">
+      <c r="B234" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="C234" s="80" t="s">
+      <c r="C234" s="81" t="s">
         <v>90</v>
       </c>
       <c r="D234" s="49" t="s">
@@ -11319,9 +11325,9 @@
       </c>
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A235" s="76"/>
-      <c r="B235" s="78"/>
-      <c r="C235" s="80"/>
+      <c r="A235" s="77"/>
+      <c r="B235" s="79"/>
+      <c r="C235" s="81"/>
       <c r="D235" s="49" t="s">
         <v>197</v>
       </c>
@@ -11354,9 +11360,9 @@
       </c>
     </row>
     <row r="236" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A236" s="76"/>
-      <c r="B236" s="78"/>
-      <c r="C236" s="80"/>
+      <c r="A236" s="77"/>
+      <c r="B236" s="79"/>
+      <c r="C236" s="81"/>
       <c r="D236" s="49" t="s">
         <v>199</v>
       </c>
@@ -11390,9 +11396,9 @@
       </c>
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A237" s="76"/>
-      <c r="B237" s="78"/>
-      <c r="C237" s="80"/>
+      <c r="A237" s="77"/>
+      <c r="B237" s="79"/>
+      <c r="C237" s="81"/>
       <c r="D237" s="49" t="s">
         <v>200</v>
       </c>
@@ -11425,9 +11431,9 @@
       </c>
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A238" s="76"/>
-      <c r="B238" s="78"/>
-      <c r="C238" s="80"/>
+      <c r="A238" s="77"/>
+      <c r="B238" s="79"/>
+      <c r="C238" s="81"/>
       <c r="D238" s="49" t="s">
         <v>202</v>
       </c>
@@ -11457,9 +11463,9 @@
       </c>
     </row>
     <row r="239" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A239" s="76"/>
-      <c r="B239" s="79"/>
-      <c r="C239" s="80"/>
+      <c r="A239" s="77"/>
+      <c r="B239" s="80"/>
+      <c r="C239" s="81"/>
       <c r="D239" s="49" t="s">
         <v>203</v>
       </c>
@@ -11474,13 +11480,13 @@
       </c>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A240" s="76" t="s">
+      <c r="A240" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B240" s="77" t="s">
+      <c r="B240" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="C240" s="80" t="s">
+      <c r="C240" s="81" t="s">
         <v>94</v>
       </c>
       <c r="D240" s="49" t="s">
@@ -11508,9 +11514,9 @@
       </c>
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A241" s="76"/>
-      <c r="B241" s="78"/>
-      <c r="C241" s="80"/>
+      <c r="A241" s="77"/>
+      <c r="B241" s="79"/>
+      <c r="C241" s="81"/>
       <c r="D241" s="49" t="s">
         <v>197</v>
       </c>
@@ -11539,9 +11545,9 @@
       </c>
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A242" s="76"/>
-      <c r="B242" s="78"/>
-      <c r="C242" s="80"/>
+      <c r="A242" s="77"/>
+      <c r="B242" s="79"/>
+      <c r="C242" s="81"/>
       <c r="D242" s="49" t="s">
         <v>199</v>
       </c>
@@ -11570,9 +11576,9 @@
       </c>
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A243" s="76"/>
-      <c r="B243" s="78"/>
-      <c r="C243" s="80"/>
+      <c r="A243" s="77"/>
+      <c r="B243" s="79"/>
+      <c r="C243" s="81"/>
       <c r="D243" s="49" t="s">
         <v>200</v>
       </c>
@@ -11601,9 +11607,9 @@
       </c>
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A244" s="76"/>
-      <c r="B244" s="78"/>
-      <c r="C244" s="80"/>
+      <c r="A244" s="77"/>
+      <c r="B244" s="79"/>
+      <c r="C244" s="81"/>
       <c r="D244" s="49" t="s">
         <v>202</v>
       </c>
@@ -11629,9 +11635,9 @@
       </c>
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A245" s="76"/>
-      <c r="B245" s="79"/>
-      <c r="C245" s="80"/>
+      <c r="A245" s="77"/>
+      <c r="B245" s="80"/>
+      <c r="C245" s="81"/>
       <c r="D245" s="49" t="s">
         <v>203</v>
       </c>
@@ -11644,13 +11650,13 @@
       <c r="P245" s="55"/>
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A246" s="76" t="s">
+      <c r="A246" s="77" t="s">
         <v>243</v>
       </c>
-      <c r="B246" s="77" t="s">
+      <c r="B246" s="78" t="s">
         <v>245</v>
       </c>
-      <c r="C246" s="80" t="s">
+      <c r="C246" s="81" t="s">
         <v>244</v>
       </c>
       <c r="D246" s="49" t="s">
@@ -11670,9 +11676,9 @@
       <c r="P246" s="55"/>
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A247" s="76"/>
-      <c r="B247" s="78"/>
-      <c r="C247" s="80"/>
+      <c r="A247" s="77"/>
+      <c r="B247" s="79"/>
+      <c r="C247" s="81"/>
       <c r="D247" s="49" t="s">
         <v>196</v>
       </c>
@@ -11702,9 +11708,9 @@
       </c>
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A248" s="76"/>
-      <c r="B248" s="78"/>
-      <c r="C248" s="80"/>
+      <c r="A248" s="77"/>
+      <c r="B248" s="79"/>
+      <c r="C248" s="81"/>
       <c r="D248" s="49" t="s">
         <v>196</v>
       </c>
@@ -11734,9 +11740,9 @@
       </c>
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A249" s="76"/>
-      <c r="B249" s="78"/>
-      <c r="C249" s="80"/>
+      <c r="A249" s="77"/>
+      <c r="B249" s="79"/>
+      <c r="C249" s="81"/>
       <c r="D249" s="49" t="s">
         <v>197</v>
       </c>
@@ -11766,9 +11772,9 @@
       </c>
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A250" s="76"/>
-      <c r="B250" s="78"/>
-      <c r="C250" s="80"/>
+      <c r="A250" s="77"/>
+      <c r="B250" s="79"/>
+      <c r="C250" s="81"/>
       <c r="D250" s="49" t="s">
         <v>199</v>
       </c>
@@ -11798,9 +11804,9 @@
       </c>
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A251" s="76"/>
-      <c r="B251" s="78"/>
-      <c r="C251" s="80"/>
+      <c r="A251" s="77"/>
+      <c r="B251" s="79"/>
+      <c r="C251" s="81"/>
       <c r="D251" s="49" t="s">
         <v>267</v>
       </c>
@@ -11830,9 +11836,9 @@
       </c>
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A252" s="76"/>
-      <c r="B252" s="78"/>
-      <c r="C252" s="80"/>
+      <c r="A252" s="77"/>
+      <c r="B252" s="79"/>
+      <c r="C252" s="81"/>
       <c r="D252" s="49" t="s">
         <v>200</v>
       </c>
@@ -11865,9 +11871,9 @@
       </c>
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A253" s="76"/>
-      <c r="B253" s="78"/>
-      <c r="C253" s="80"/>
+      <c r="A253" s="77"/>
+      <c r="B253" s="79"/>
+      <c r="C253" s="81"/>
       <c r="D253" s="49" t="s">
         <v>265</v>
       </c>
@@ -11898,9 +11904,9 @@
       </c>
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A254" s="76"/>
-      <c r="B254" s="79"/>
-      <c r="C254" s="80"/>
+      <c r="A254" s="77"/>
+      <c r="B254" s="80"/>
+      <c r="C254" s="81"/>
       <c r="D254" s="49" t="s">
         <v>203</v>
       </c>
@@ -11917,13 +11923,13 @@
       </c>
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A255" s="76" t="s">
+      <c r="A255" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="B255" s="77" t="s">
+      <c r="B255" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="C255" s="80" t="s">
+      <c r="C255" s="81" t="s">
         <v>97</v>
       </c>
       <c r="D255" s="49" t="s">
@@ -11949,9 +11955,9 @@
       </c>
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A256" s="76"/>
-      <c r="B256" s="78"/>
-      <c r="C256" s="80"/>
+      <c r="A256" s="77"/>
+      <c r="B256" s="79"/>
+      <c r="C256" s="81"/>
       <c r="D256" s="49" t="s">
         <v>197</v>
       </c>
@@ -11978,9 +11984,9 @@
       </c>
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A257" s="76"/>
-      <c r="B257" s="78"/>
-      <c r="C257" s="80"/>
+      <c r="A257" s="77"/>
+      <c r="B257" s="79"/>
+      <c r="C257" s="81"/>
       <c r="D257" s="49" t="s">
         <v>199</v>
       </c>
@@ -12007,9 +12013,9 @@
       </c>
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A258" s="76"/>
-      <c r="B258" s="78"/>
-      <c r="C258" s="80"/>
+      <c r="A258" s="77"/>
+      <c r="B258" s="79"/>
+      <c r="C258" s="81"/>
       <c r="D258" s="49" t="s">
         <v>200</v>
       </c>
@@ -12036,9 +12042,9 @@
       </c>
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A259" s="76"/>
-      <c r="B259" s="78"/>
-      <c r="C259" s="80"/>
+      <c r="A259" s="77"/>
+      <c r="B259" s="79"/>
+      <c r="C259" s="81"/>
       <c r="D259" s="49" t="s">
         <v>202</v>
       </c>
@@ -12062,9 +12068,9 @@
       </c>
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A260" s="76"/>
-      <c r="B260" s="79"/>
-      <c r="C260" s="80"/>
+      <c r="A260" s="77"/>
+      <c r="B260" s="80"/>
+      <c r="C260" s="81"/>
       <c r="D260" s="49" t="s">
         <v>203</v>
       </c>
@@ -12077,13 +12083,13 @@
       <c r="P260" s="55"/>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A261" s="76" t="s">
+      <c r="A261" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="B261" s="77" t="s">
+      <c r="B261" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="C261" s="80" t="s">
+      <c r="C261" s="81" t="s">
         <v>100</v>
       </c>
       <c r="D261" s="49" t="s">
@@ -12113,9 +12119,9 @@
       <c r="P261" s="55"/>
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A262" s="76"/>
-      <c r="B262" s="78"/>
-      <c r="C262" s="80"/>
+      <c r="A262" s="77"/>
+      <c r="B262" s="79"/>
+      <c r="C262" s="81"/>
       <c r="D262" s="49" t="s">
         <v>197</v>
       </c>
@@ -12146,9 +12152,9 @@
       <c r="P262" s="55"/>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A263" s="76"/>
-      <c r="B263" s="78"/>
-      <c r="C263" s="80"/>
+      <c r="A263" s="77"/>
+      <c r="B263" s="79"/>
+      <c r="C263" s="81"/>
       <c r="D263" s="49" t="s">
         <v>199</v>
       </c>
@@ -12179,9 +12185,9 @@
       <c r="P263" s="55"/>
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A264" s="76"/>
-      <c r="B264" s="78"/>
-      <c r="C264" s="80"/>
+      <c r="A264" s="77"/>
+      <c r="B264" s="79"/>
+      <c r="C264" s="81"/>
       <c r="D264" s="49" t="s">
         <v>200</v>
       </c>
@@ -12202,9 +12208,9 @@
       <c r="P264" s="55"/>
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A265" s="76"/>
-      <c r="B265" s="78"/>
-      <c r="C265" s="80"/>
+      <c r="A265" s="77"/>
+      <c r="B265" s="79"/>
+      <c r="C265" s="81"/>
       <c r="D265" s="49" t="s">
         <v>202</v>
       </c>
@@ -12232,9 +12238,9 @@
       <c r="P265" s="55"/>
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A266" s="76"/>
-      <c r="B266" s="79"/>
-      <c r="C266" s="80"/>
+      <c r="A266" s="77"/>
+      <c r="B266" s="80"/>
+      <c r="C266" s="81"/>
       <c r="D266" s="49" t="s">
         <v>203</v>
       </c>
@@ -12247,13 +12253,13 @@
       <c r="P266" s="55"/>
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A267" s="76" t="s">
+      <c r="A267" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B267" s="77" t="s">
+      <c r="B267" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="C267" s="80" t="s">
+      <c r="C267" s="81" t="s">
         <v>103</v>
       </c>
       <c r="D267" s="49" t="s">
@@ -12283,9 +12289,9 @@
       <c r="P267" s="55"/>
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A268" s="76"/>
-      <c r="B268" s="78"/>
-      <c r="C268" s="80"/>
+      <c r="A268" s="77"/>
+      <c r="B268" s="79"/>
+      <c r="C268" s="81"/>
       <c r="D268" s="49" t="s">
         <v>197</v>
       </c>
@@ -12316,9 +12322,9 @@
       <c r="P268" s="55"/>
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A269" s="76"/>
-      <c r="B269" s="78"/>
-      <c r="C269" s="80"/>
+      <c r="A269" s="77"/>
+      <c r="B269" s="79"/>
+      <c r="C269" s="81"/>
       <c r="D269" s="49" t="s">
         <v>199</v>
       </c>
@@ -12349,9 +12355,9 @@
       <c r="P269" s="55"/>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A270" s="76"/>
-      <c r="B270" s="78"/>
-      <c r="C270" s="80"/>
+      <c r="A270" s="77"/>
+      <c r="B270" s="79"/>
+      <c r="C270" s="81"/>
       <c r="D270" s="49" t="s">
         <v>200</v>
       </c>
@@ -12372,9 +12378,9 @@
       <c r="P270" s="55"/>
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A271" s="76"/>
-      <c r="B271" s="78"/>
-      <c r="C271" s="80"/>
+      <c r="A271" s="77"/>
+      <c r="B271" s="79"/>
+      <c r="C271" s="81"/>
       <c r="D271" s="49" t="s">
         <v>202</v>
       </c>
@@ -12402,9 +12408,9 @@
       <c r="P271" s="55"/>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A272" s="76"/>
-      <c r="B272" s="79"/>
-      <c r="C272" s="80"/>
+      <c r="A272" s="77"/>
+      <c r="B272" s="80"/>
+      <c r="C272" s="81"/>
       <c r="D272" s="49" t="s">
         <v>203</v>
       </c>
@@ -12417,13 +12423,13 @@
       <c r="P272" s="55"/>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A273" s="76" t="s">
+      <c r="A273" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B273" s="77" t="s">
+      <c r="B273" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="C273" s="80" t="s">
+      <c r="C273" s="81" t="s">
         <v>103</v>
       </c>
       <c r="D273" s="49" t="s">
@@ -12449,9 +12455,9 @@
       </c>
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A274" s="76"/>
-      <c r="B274" s="78"/>
-      <c r="C274" s="80"/>
+      <c r="A274" s="77"/>
+      <c r="B274" s="79"/>
+      <c r="C274" s="81"/>
       <c r="D274" s="49" t="s">
         <v>197</v>
       </c>
@@ -12478,9 +12484,9 @@
       </c>
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A275" s="76"/>
-      <c r="B275" s="78"/>
-      <c r="C275" s="80"/>
+      <c r="A275" s="77"/>
+      <c r="B275" s="79"/>
+      <c r="C275" s="81"/>
       <c r="D275" s="49" t="s">
         <v>200</v>
       </c>
@@ -12501,9 +12507,9 @@
       <c r="P275" s="55"/>
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A276" s="76"/>
-      <c r="B276" s="78"/>
-      <c r="C276" s="80"/>
+      <c r="A276" s="77"/>
+      <c r="B276" s="79"/>
+      <c r="C276" s="81"/>
       <c r="D276" s="49" t="s">
         <v>202</v>
       </c>
@@ -12523,9 +12529,9 @@
       </c>
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A277" s="76"/>
-      <c r="B277" s="78"/>
-      <c r="C277" s="80"/>
+      <c r="A277" s="77"/>
+      <c r="B277" s="79"/>
+      <c r="C277" s="81"/>
       <c r="D277" s="49" t="s">
         <v>274</v>
       </c>
@@ -12542,9 +12548,9 @@
       </c>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A278" s="76"/>
-      <c r="B278" s="79"/>
-      <c r="C278" s="80"/>
+      <c r="A278" s="77"/>
+      <c r="B278" s="80"/>
+      <c r="C278" s="81"/>
       <c r="D278" s="49" t="s">
         <v>203</v>
       </c>
@@ -12562,6 +12568,71 @@
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="A165:A180"/>
+    <mergeCell ref="A273:A278"/>
+    <mergeCell ref="B273:B278"/>
+    <mergeCell ref="C273:C278"/>
+    <mergeCell ref="C255:C260"/>
+    <mergeCell ref="C261:C266"/>
+    <mergeCell ref="C267:C272"/>
+    <mergeCell ref="C146:C164"/>
+    <mergeCell ref="C140:C145"/>
+    <mergeCell ref="C218:C233"/>
+    <mergeCell ref="C53:C65"/>
+    <mergeCell ref="B267:B272"/>
+    <mergeCell ref="C165:C180"/>
+    <mergeCell ref="C197:C204"/>
+    <mergeCell ref="C205:C210"/>
+    <mergeCell ref="C234:C239"/>
+    <mergeCell ref="C240:C245"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="B255:B260"/>
+    <mergeCell ref="B261:B266"/>
+    <mergeCell ref="B197:B204"/>
+    <mergeCell ref="B205:B210"/>
+    <mergeCell ref="B234:B239"/>
+    <mergeCell ref="B240:B245"/>
+    <mergeCell ref="B218:B233"/>
+    <mergeCell ref="B146:B164"/>
+    <mergeCell ref="B211:B217"/>
+    <mergeCell ref="B246:B254"/>
+    <mergeCell ref="B130:B139"/>
+    <mergeCell ref="B53:B65"/>
+    <mergeCell ref="B165:B180"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="C211:C217"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="B140:B145"/>
+    <mergeCell ref="A255:A260"/>
+    <mergeCell ref="A261:A266"/>
+    <mergeCell ref="A267:A272"/>
+    <mergeCell ref="A197:A204"/>
+    <mergeCell ref="A205:A210"/>
+    <mergeCell ref="A234:A239"/>
+    <mergeCell ref="A240:A245"/>
+    <mergeCell ref="A218:A233"/>
+    <mergeCell ref="A211:A217"/>
+    <mergeCell ref="A181:A196"/>
+    <mergeCell ref="A53:A65"/>
+    <mergeCell ref="A146:A164"/>
+    <mergeCell ref="A140:A145"/>
+    <mergeCell ref="A130:A139"/>
+    <mergeCell ref="A246:A254"/>
+    <mergeCell ref="C121:C129"/>
+    <mergeCell ref="C130:C139"/>
+    <mergeCell ref="C246:C254"/>
+    <mergeCell ref="A23:A46"/>
+    <mergeCell ref="B23:B46"/>
+    <mergeCell ref="C23:C46"/>
+    <mergeCell ref="A95:A102"/>
+    <mergeCell ref="B95:B102"/>
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="A103:A111"/>
+    <mergeCell ref="B103:B111"/>
+    <mergeCell ref="C103:C111"/>
+    <mergeCell ref="A112:A120"/>
+    <mergeCell ref="B112:B120"/>
+    <mergeCell ref="C112:C120"/>
     <mergeCell ref="A2:A22"/>
     <mergeCell ref="B2:B22"/>
     <mergeCell ref="C2:C22"/>
@@ -12578,71 +12649,6 @@
     <mergeCell ref="A66:A78"/>
     <mergeCell ref="B66:B78"/>
     <mergeCell ref="C66:C78"/>
-    <mergeCell ref="A246:A254"/>
-    <mergeCell ref="C121:C129"/>
-    <mergeCell ref="C130:C139"/>
-    <mergeCell ref="C246:C254"/>
-    <mergeCell ref="A23:A46"/>
-    <mergeCell ref="B23:B46"/>
-    <mergeCell ref="C23:C46"/>
-    <mergeCell ref="A95:A102"/>
-    <mergeCell ref="B95:B102"/>
-    <mergeCell ref="C95:C102"/>
-    <mergeCell ref="A103:A111"/>
-    <mergeCell ref="B103:B111"/>
-    <mergeCell ref="C103:C111"/>
-    <mergeCell ref="A112:A120"/>
-    <mergeCell ref="B112:B120"/>
-    <mergeCell ref="C112:C120"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="B140:B145"/>
-    <mergeCell ref="A255:A260"/>
-    <mergeCell ref="A261:A266"/>
-    <mergeCell ref="A267:A272"/>
-    <mergeCell ref="A197:A204"/>
-    <mergeCell ref="A205:A210"/>
-    <mergeCell ref="A234:A239"/>
-    <mergeCell ref="A240:A245"/>
-    <mergeCell ref="A218:A233"/>
-    <mergeCell ref="A211:A217"/>
-    <mergeCell ref="A181:A196"/>
-    <mergeCell ref="A53:A65"/>
-    <mergeCell ref="A146:A164"/>
-    <mergeCell ref="A140:A145"/>
-    <mergeCell ref="A130:A139"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="B255:B260"/>
-    <mergeCell ref="B261:B266"/>
-    <mergeCell ref="B197:B204"/>
-    <mergeCell ref="B205:B210"/>
-    <mergeCell ref="B234:B239"/>
-    <mergeCell ref="B240:B245"/>
-    <mergeCell ref="B218:B233"/>
-    <mergeCell ref="B146:B164"/>
-    <mergeCell ref="B211:B217"/>
-    <mergeCell ref="B246:B254"/>
-    <mergeCell ref="B130:B139"/>
-    <mergeCell ref="B53:B65"/>
-    <mergeCell ref="B165:B180"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="C211:C217"/>
-    <mergeCell ref="C146:C164"/>
-    <mergeCell ref="C140:C145"/>
-    <mergeCell ref="C218:C233"/>
-    <mergeCell ref="C53:C65"/>
-    <mergeCell ref="B267:B272"/>
-    <mergeCell ref="C165:C180"/>
-    <mergeCell ref="C197:C204"/>
-    <mergeCell ref="C205:C210"/>
-    <mergeCell ref="C234:C239"/>
-    <mergeCell ref="C240:C245"/>
-    <mergeCell ref="A165:A180"/>
-    <mergeCell ref="A273:A278"/>
-    <mergeCell ref="B273:B278"/>
-    <mergeCell ref="C273:C278"/>
-    <mergeCell ref="C255:C260"/>
-    <mergeCell ref="C261:C266"/>
-    <mergeCell ref="C267:C272"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P196" r:id="rId1" xr:uid="{1E4E8135-CD07-B347-936C-A97039970762}"/>
@@ -12795,41 +12801,40 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="84">
+      <c r="H3">
         <v>2021</v>
       </c>
-      <c r="I3" s="87">
+      <c r="I3" s="39">
         <v>2020</v>
       </c>
-      <c r="J3" s="88">
+      <c r="J3" s="76">
         <v>4386675.8489898499</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" t="s">
         <v>207</v>
       </c>
-      <c r="L3" s="84">
+      <c r="L3">
         <v>2050</v>
       </c>
-      <c r="M3" s="89">
+      <c r="M3" s="41">
         <v>0.85</v>
       </c>
     </row>
@@ -15632,7 +15637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>